<commit_message>
fix final project. But actually there's still need maintenance but I don't care
</commit_message>
<xml_diff>
--- a/client/public/Template Personal Data.xlsx
+++ b/client/public/Template Personal Data.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>3517082206780000</t>
   </si>
@@ -102,6 +102,9 @@
     <t>GARENG@GMAIL.COM</t>
   </si>
   <si>
+    <t>TETAP</t>
+  </si>
+  <si>
     <t>3517082206780001</t>
   </si>
   <si>
@@ -114,6 +117,9 @@
     <t>ASISTEN MANAJER SDM</t>
   </si>
   <si>
+    <t>7/24/1981</t>
+  </si>
+  <si>
     <t>0813325755569</t>
   </si>
   <si>
@@ -132,6 +138,9 @@
     <t>JOMBANG</t>
   </si>
   <si>
+    <t>1/1/2983</t>
+  </si>
+  <si>
     <t>PERUM PULO ASRI BLOK G - 5 JOMBANG</t>
   </si>
   <si>
@@ -141,6 +150,9 @@
     <t>ATENG@GMAIL.COM</t>
   </si>
   <si>
+    <t>TIDAK TETAP</t>
+  </si>
+  <si>
     <t>3517082206780003</t>
   </si>
   <si>
@@ -151,6 +163,9 @@
   </si>
   <si>
     <t>JAKARTA</t>
+  </si>
+  <si>
+    <t>5/5/1987</t>
   </si>
   <si>
     <t>0813325755561</t>
@@ -164,14 +179,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="00000000"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="dd\.mm\.yyyy"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="00000000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -187,6 +202,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -196,9 +218,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -210,30 +232,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -245,6 +247,14 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -253,14 +263,48 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -275,26 +319,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Mangal"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -306,28 +339,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -336,14 +347,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Mangal"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -352,12 +373,6 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -368,13 +383,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,169 +539,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,17 +577,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,26 +610,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -636,11 +625,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -662,176 +677,176 @@
   </borders>
   <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="179" fontId="23" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="178" fontId="18" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
@@ -862,6 +877,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="78">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1502,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="3"/>
@@ -1561,28 +1577,31 @@
       <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N1" s="9"/>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7">
-        <v>29791</v>
+      <c r="F2" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -1597,30 +1616,33 @@
         <v>9</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="7">
-        <v>395560</v>
+        <v>23</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
@@ -1632,33 +1654,36 @@
         <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="7">
-        <v>31902</v>
+        <v>32</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
@@ -1673,10 +1698,13 @@
         <v>9</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>